<commit_message>
Sistemato il thread di invio dei messaggi
</commit_message>
<xml_diff>
--- a/numeri.xlsx
+++ b/numeri.xlsx
@@ -1,41 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GiovanniPio\Desktop\Hermes repo\Hermes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCB6BF35-EFF6-4B90-B824-FA1D6479EAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38998D33-CB6F-40B0-A130-5EFEB2E024D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="855" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="-19320" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>+393802857952</t>
-  </si>
-  <si>
-    <t>+393466296727</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>questo messaggio viene da excel</t>
   </si>
@@ -43,20 +28,14 @@
     <t>ammaccabanane</t>
   </si>
   <si>
-    <t>+39 a 789</t>
-  </si>
-  <si>
-    <t>+3270386536</t>
-  </si>
-  <si>
-    <t>33350364ice</t>
+    <t>+39 346 629 6727</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +47,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,11 +357,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,40 +373,44 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,6 +429,7 @@
       <c r="D12" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>